<commit_message>
updated layout, credit | jackpot | bet label added
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Game Object</t>
   </si>
@@ -70,15 +70,44 @@
   </si>
   <si>
     <t>Quit</t>
+  </si>
+  <si>
+    <t>creditImage</t>
+  </si>
+  <si>
+    <t>betImage</t>
+  </si>
+  <si>
+    <t>jackpot label</t>
+  </si>
+  <si>
+    <t>credit label</t>
+  </si>
+  <si>
+    <t>bet label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,15 +162,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -413,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,18 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.875" style="1"/>
-    <col min="4" max="4" width="13.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
@@ -626,18 +660,147 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>80</v>
+      </c>
+      <c r="C12" s="2">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2">
+        <v>180</v>
+      </c>
+      <c r="E12" s="2">
+        <v>293</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>335</v>
+      </c>
+      <c r="E13" s="2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>290</v>
+      </c>
+      <c r="E15" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7">
+        <v>433</v>
+      </c>
+      <c r="E16" s="7">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Functional game play on Console
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -446,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,7 +457,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
@@ -703,7 +703,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -716,7 +716,7 @@
         <v>290</v>
       </c>
       <c r="E15" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -729,7 +729,7 @@
         <v>433</v>
       </c>
       <c r="E16" s="7">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>

<commit_message>
updated UI for message box
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Game Object</t>
   </si>
@@ -85,15 +85,46 @@
   </si>
   <si>
     <t>bet label</t>
+  </si>
+  <si>
+    <t>RanOutMoney Message</t>
+  </si>
+  <si>
+    <t>NotEnoughMoney</t>
+  </si>
+  <si>
+    <t>OK button</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>QuitMessage</t>
+  </si>
+  <si>
+    <t>YES button</t>
+  </si>
+  <si>
+    <t>NO button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,20 +193,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,13 +494,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.25" style="1" customWidth="1"/>
@@ -733,60 +771,138 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="7">
+        <v>300</v>
+      </c>
+      <c r="C17" s="7">
+        <v>100</v>
+      </c>
+      <c r="D17" s="7">
+        <v>166</v>
+      </c>
+      <c r="E17" s="7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="9" customFormat="1">
+      <c r="A18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="7">
+        <v>300</v>
+      </c>
+      <c r="C18" s="7">
+        <v>100</v>
+      </c>
+      <c r="D18" s="7">
+        <v>166</v>
+      </c>
+      <c r="E18" s="7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="9" customFormat="1">
+      <c r="A19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7">
+        <v>60</v>
+      </c>
+      <c r="C19" s="7">
+        <v>40</v>
+      </c>
+      <c r="D19" s="7">
+        <v>220</v>
+      </c>
+      <c r="E19" s="7">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="9" customFormat="1">
+      <c r="A20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7">
+        <v>70</v>
+      </c>
+      <c r="C20" s="7">
+        <v>40</v>
+      </c>
+      <c r="D20" s="7">
+        <v>350</v>
+      </c>
+      <c r="E20" s="7">
+        <v>243</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7">
+        <v>40</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7">
+        <v>243</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="7">
+        <v>300</v>
+      </c>
+      <c r="C22" s="7">
+        <v>100</v>
+      </c>
+      <c r="D22" s="7">
+        <v>166</v>
+      </c>
+      <c r="E22" s="7">
+        <v>190</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="7">
+        <v>50</v>
+      </c>
+      <c r="C23" s="7">
+        <v>50</v>
+      </c>
+      <c r="D23" s="7">
+        <v>220</v>
+      </c>
+      <c r="E23" s="7">
+        <v>235</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="7">
+        <v>50</v>
+      </c>
+      <c r="C24" s="7">
+        <v>50</v>
+      </c>
+      <c r="D24" s="7">
+        <v>350</v>
+      </c>
+      <c r="E24" s="7">
+        <v>235</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6"/>

</xml_diff>

<commit_message>
win and totalWin counter added
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Game Object</t>
   </si>
@@ -109,15 +109,34 @@
   </si>
   <si>
     <t>NO button</t>
+  </si>
+  <si>
+    <t>win image</t>
+  </si>
+  <si>
+    <t>total win image</t>
+  </si>
+  <si>
+    <t>win label</t>
+  </si>
+  <si>
+    <t>total win label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -193,27 +212,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -492,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
@@ -905,18 +928,64 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="7">
+        <v>80</v>
+      </c>
+      <c r="C25" s="7">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7">
+        <v>172</v>
+      </c>
+      <c r="E25" s="7">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="7">
+        <v>80</v>
+      </c>
+      <c r="C26" s="7">
+        <v>35</v>
+      </c>
+      <c r="D26" s="7">
+        <v>330</v>
+      </c>
+      <c r="E26" s="7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12">
+        <v>270</v>
+      </c>
+      <c r="E27" s="12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12">
+        <v>420</v>
+      </c>
+      <c r="E28" s="12">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>